<commit_message>
this is an interesting fit -- testing more model runs, hard to get a good fit for juv, spawners, and survival rates that make sense
this fit has a bit more variation than i would like, but it generally is OK, a little tweaking from here may be good.

starting values best when only assigning by age (rather than blanket across the whole 1:5 timeseries)

added p_2 t+1, wasn't like this before, just p_2 -- removed for now, doesnt make a difference?

removed the 0.1 on starting values so they arent forced, re-running. things got weird at time step 11 with starting values I think propogating forward.
</commit_message>
<xml_diff>
--- a/survival test excel.xlsx
+++ b/survival test excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AC96803-DD93-A14D-9AA1-489AAC7D64A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC388DFC-4DF6-614C-A61B-C416BB5F0900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="760" windowWidth="29600" windowHeight="20040" xr2:uid="{43972CCF-D74D-C149-826D-0934E9C72141}"/>
+    <workbookView xWindow="2160" yWindow="4460" windowWidth="26880" windowHeight="17920" xr2:uid="{43972CCF-D74D-C149-826D-0934E9C72141}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>c</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t xml:space="preserve"> increase productivity, survival goes up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if C is similar to N_eggs or slightly larger, then  survival is normal ish. </t>
+  </si>
+  <si>
+    <t>if n_eggs &gt; C, survival gets really small</t>
   </si>
 </sst>
 </file>
@@ -175,13 +181,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -520,13 +525,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE4AB08-0461-6945-9305-D6B5CB914DA4}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -564,38 +575,38 @@
         <f>EXP(15)</f>
         <v>3269017.3724721107</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3">
         <v>0.08</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <f>EXP(14)</f>
         <v>1202604.2841647768</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f>B3/(1+(B3+C3)/A3)</f>
         <v>5.8484685244074207E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <f>EXP(10)</f>
         <v>22026.465794806718</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.08</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <f>EXP(14)</f>
         <v>1202604.2841647768</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <f t="shared" ref="D4:D7" si="0">B4/(1+(B4+C4)/A4)</f>
         <v>1.438896702970227E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f t="shared" ref="A4:A9" si="1">EXP(15)</f>
+        <f t="shared" ref="A5:A9" si="1">EXP(15)</f>
         <v>3269017.3724721107</v>
       </c>
       <c r="B5" s="2">
@@ -615,14 +626,14 @@
         <f>EXP(10)</f>
         <v>22026.465794806718</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>0.08</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6">
         <f>EXP(20)</f>
         <v>485165195.40979028</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>3.6318294955959187E-6</v>
       </c>
@@ -635,14 +646,14 @@
         <f t="shared" si="1"/>
         <v>3269017.3724721107</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>0.08</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7">
         <f>EXP(10)</f>
         <v>22026.465794806718</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>7.9464569994400894E-2</v>
       </c>
@@ -651,18 +662,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <f t="shared" si="1"/>
         <v>3269017.3724721107</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>0.08</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <f>EXP(15)</f>
         <v>3269017.3724721107</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <f t="shared" ref="D8:D9" si="2">B8/(1+(B8+C8)/A8)</f>
         <v>3.9999999510556293E-2</v>
       </c>
@@ -675,19 +686,110 @@
         <f t="shared" si="1"/>
         <v>3269017.3724721107</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>0.3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9">
         <f>EXP(10)</f>
         <v>22026.465794806718</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f t="shared" si="2"/>
         <v>0.29799211755879951</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>EXP(15)</f>
+        <v>3269017.3724721107</v>
+      </c>
+      <c r="B12">
+        <v>0.27</v>
+      </c>
+      <c r="C12">
+        <f>EXP(13.7)</f>
+        <v>890911.16597916035</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" ref="D12" si="3">B12/(1+(B12+C12)/A12)</f>
+        <v>0.21217543165025274</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f>EXP(15)</f>
+        <v>3269017.3724721107</v>
+      </c>
+      <c r="B13">
+        <v>0.27</v>
+      </c>
+      <c r="C13">
+        <f>EXP(20)</f>
+        <v>485165195.40979028</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:D14" si="4">B13/(1+(B13+C13)/A13)</f>
+        <v>1.8070697485579868E-3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f>EXP(15)</f>
+        <v>3269017.3724721107</v>
+      </c>
+      <c r="B14">
+        <v>0.27</v>
+      </c>
+      <c r="C14">
+        <f>EXP(14)</f>
+        <v>1202604.2841647768</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="4"/>
+        <v>0.19738580431179265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f>EXP(15)</f>
+        <v>3269017.3724721107</v>
+      </c>
+      <c r="B15">
+        <v>0.27</v>
+      </c>
+      <c r="C15">
+        <f>EXP(25)</f>
+        <v>72004899337.38588</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" ref="D15" si="5">B15/(1+(B15+C15)/A15)</f>
+        <v>1.2257424549611325E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f>EXP(14)</f>
+        <v>1202604.2841647768</v>
+      </c>
+      <c r="B18">
+        <v>0.75</v>
+      </c>
+      <c r="C18">
+        <f>EXP(15)</f>
+        <v>3269017.3724721107</v>
+      </c>
+      <c r="D18" s="8">
+        <f t="shared" ref="D18" si="6">B18/(1+(B18+C18)/A18)</f>
+        <v>0.20170603219647582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>